<commit_message>
6-Excel Data Cleaning Excel Tutorial
</commit_message>
<xml_diff>
--- a/Data Cleaning Excel Tutorial.xlsx
+++ b/Data Cleaning Excel Tutorial.xlsx
@@ -1,21 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/579481080490e445/Documents/Excel Series Excels/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{C3F4832D-6691-4E80-9CE5-51C600B1F941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4506"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="US_Presidents Excel Tutorial Da" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'US_Presidents Excel Tutorial Da'!$E$1:$E$48</definedName>
+  </definedNames>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="132">
   <si>
     <t>S.No.</t>
   </si>
@@ -58,9 +55,6 @@
     <t>John Adams</t>
   </si>
   <si>
-    <t>john adams</t>
-  </si>
-  <si>
     <t>1st  Vice President of the United States</t>
   </si>
   <si>
@@ -76,21 +70,12 @@
     <t>Democratic-  Republican</t>
   </si>
   <si>
-    <t xml:space="preserve">    Aaron Burr</t>
-  </si>
-  <si>
     <t>James Madison</t>
   </si>
   <si>
     <t>5th  United States Secretary of State   (1801â€“1809)</t>
   </si>
   <si>
-    <t>George    Clinton</t>
-  </si>
-  <si>
-    <t>JAMES MONROE</t>
-  </si>
-  <si>
     <t>7th  United States Secretary of State   (1811â€“1817)</t>
   </si>
   <si>
@@ -115,9 +100,6 @@
     <t>Democratic</t>
   </si>
   <si>
-    <t>John C.     Calhoun</t>
-  </si>
-  <si>
     <t>Martin Van Buren</t>
   </si>
   <si>
@@ -139,15 +121,9 @@
     <t>John Tyler</t>
   </si>
   <si>
-    <t>john tyler</t>
-  </si>
-  <si>
     <t>10th  Vice President of the United States</t>
   </si>
   <si>
-    <t>Whig   April 4, 1841  â€“  September 13, 1841</t>
-  </si>
-  <si>
     <t>Office vacant</t>
   </si>
   <si>
@@ -157,18 +133,12 @@
     <t>9th  Governor of Tennessee   (1839â€“1841)</t>
   </si>
   <si>
-    <t>George         M. Dallas</t>
-  </si>
-  <si>
     <t>Zachary Taylor</t>
   </si>
   <si>
     <t>Major General  of the  1st Infantry Regiment   United States Army   (1846â€“1849)</t>
   </si>
   <si>
-    <t xml:space="preserve">               Millard Fillmore</t>
-  </si>
-  <si>
     <t>Millard Fillmore</t>
   </si>
   <si>
@@ -265,9 +235,6 @@
     <t>Adlai Stevenson</t>
   </si>
   <si>
-    <t>William McKinley</t>
-  </si>
-  <si>
     <t>39th  Governor of Ohio   (1892â€“1896)</t>
   </si>
   <si>
@@ -430,9 +397,6 @@
     <t>Nonpartisan</t>
   </si>
   <si>
-    <t>Republicans</t>
-  </si>
-  <si>
     <t>Demorcatic</t>
   </si>
   <si>
@@ -443,17 +407,31 @@
   </si>
   <si>
     <t>date updated</t>
+  </si>
+  <si>
+    <t>James Monroe</t>
+  </si>
+  <si>
+    <t>William Mckinley</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whig   </t>
+  </si>
+  <si>
+    <t>Aaron Burr</t>
+  </si>
+  <si>
+    <t>George Clinton</t>
+  </si>
+  <si>
+    <t>George M. Dallas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="179" formatCode="&quot;$&quot;#,##0.00"/>
-  </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -936,12 +914,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1043,7 +1020,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1095,7 +1072,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1289,26 +1266,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="23.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="23.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="7" max="7" width="23.5546875" style="3"/>
+    <col min="4" max="4" width="65.21875" customWidth="1"/>
+    <col min="7" max="7" width="23.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1324,17 +1302,17 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>134</v>
+      <c r="G1" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="H1" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="I1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1348,12 +1326,12 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>5000</v>
       </c>
       <c r="H2" s="1">
@@ -1363,7 +1341,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1371,18 +1349,18 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>10000</v>
       </c>
       <c r="H3" s="1">
@@ -1392,7 +1370,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1400,18 +1378,18 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
       <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="4">
+        <v>129</v>
+      </c>
+      <c r="G4" s="3">
         <v>15000</v>
       </c>
       <c r="H4" s="1">
@@ -1421,7 +1399,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1429,18 +1407,18 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="4">
+        <v>130</v>
+      </c>
+      <c r="G5" s="3">
         <v>20000</v>
       </c>
       <c r="H5" s="1">
@@ -1450,7 +1428,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1458,18 +1436,18 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>126</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="4">
+        <v>16</v>
+      </c>
+      <c r="G6" s="3">
         <v>25000</v>
       </c>
       <c r="H6" s="1">
@@ -1479,7 +1457,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1487,18 +1465,18 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="4">
+        <v>19</v>
+      </c>
+      <c r="G7" s="3">
         <v>30000</v>
       </c>
       <c r="H7" s="1">
@@ -1508,7 +1486,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1516,18 +1494,18 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="4">
+        <v>19</v>
+      </c>
+      <c r="G8" s="3">
         <v>35000</v>
       </c>
       <c r="H8" s="1">
@@ -1537,7 +1515,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1545,18 +1523,18 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="4">
+        <v>25</v>
+      </c>
+      <c r="G9" s="3">
         <v>40000</v>
       </c>
       <c r="H9" s="1">
@@ -1566,7 +1544,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1574,18 +1552,18 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="4">
+        <v>29</v>
+      </c>
+      <c r="G10" s="3">
         <v>45000</v>
       </c>
       <c r="H10" s="1">
@@ -1595,7 +1573,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1603,18 +1581,18 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>128</v>
       </c>
       <c r="F11" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="4">
+        <v>31</v>
+      </c>
+      <c r="G11" s="3">
         <v>50000</v>
       </c>
       <c r="H11" s="1">
@@ -1624,7 +1602,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1632,18 +1610,18 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G12" s="4">
+        <v>131</v>
+      </c>
+      <c r="G12" s="3">
         <v>55000</v>
       </c>
       <c r="H12" s="1">
@@ -1653,7 +1631,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1661,18 +1639,18 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F13" t="s">
-        <v>44</v>
-      </c>
-      <c r="G13" s="4">
+        <v>36</v>
+      </c>
+      <c r="G13" s="3">
         <v>60000</v>
       </c>
       <c r="H13" s="1">
@@ -1682,7 +1660,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1690,18 +1668,18 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="E14" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G14" s="4">
+        <v>31</v>
+      </c>
+      <c r="G14" s="3">
         <v>65000</v>
       </c>
       <c r="H14" s="1">
@@ -1711,7 +1689,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1719,18 +1697,18 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F15" t="s">
-        <v>49</v>
-      </c>
-      <c r="G15" s="4">
+        <v>40</v>
+      </c>
+      <c r="G15" s="3">
         <v>75000</v>
       </c>
       <c r="H15" s="1">
@@ -1740,7 +1718,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1748,18 +1726,18 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E16" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F16" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="4">
+        <v>43</v>
+      </c>
+      <c r="G16" s="3">
         <v>85000</v>
       </c>
       <c r="H16" s="1">
@@ -1769,7 +1747,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1777,18 +1755,18 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E17" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F17" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" s="4">
+        <v>46</v>
+      </c>
+      <c r="G17" s="3">
         <v>95000</v>
       </c>
       <c r="H17" s="1">
@@ -1798,7 +1776,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1806,18 +1784,18 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" s="4">
+        <v>31</v>
+      </c>
+      <c r="G18" s="3">
         <v>105000</v>
       </c>
       <c r="H18" s="1">
@@ -1827,7 +1805,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1835,18 +1813,18 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E19" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F19" t="s">
-        <v>61</v>
-      </c>
-      <c r="G19" s="4">
+        <v>52</v>
+      </c>
+      <c r="G19" s="3">
         <v>115000</v>
       </c>
       <c r="H19" s="1">
@@ -1856,7 +1834,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1864,18 +1842,18 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D20" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E20" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F20" t="s">
-        <v>64</v>
-      </c>
-      <c r="G20" s="4">
+        <v>55</v>
+      </c>
+      <c r="G20" s="3">
         <v>125000</v>
       </c>
       <c r="H20" s="1">
@@ -1885,7 +1863,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1893,18 +1871,18 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D21" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E21" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F21" t="s">
-        <v>67</v>
-      </c>
-      <c r="G21" s="4">
+        <v>58</v>
+      </c>
+      <c r="G21" s="3">
         <v>135000</v>
       </c>
       <c r="H21" s="1">
@@ -1914,7 +1892,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1922,18 +1900,18 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D22" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E22" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F22" t="s">
-        <v>38</v>
-      </c>
-      <c r="G22" s="4">
+        <v>31</v>
+      </c>
+      <c r="G22" s="3">
         <v>145000</v>
       </c>
       <c r="H22" s="1">
@@ -1943,7 +1921,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1951,18 +1929,18 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D23" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E23" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F23" t="s">
-        <v>71</v>
-      </c>
-      <c r="G23" s="4">
+        <v>62</v>
+      </c>
+      <c r="G23" s="3">
         <v>155000</v>
       </c>
       <c r="H23" s="1">
@@ -1972,7 +1950,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1980,18 +1958,18 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E24" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F24" t="s">
-        <v>74</v>
-      </c>
-      <c r="G24" s="4">
+        <v>65</v>
+      </c>
+      <c r="G24" s="3">
         <v>165000</v>
       </c>
       <c r="H24" s="1">
@@ -2001,7 +1979,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2009,18 +1987,18 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D25" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E25" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F25" t="s">
-        <v>76</v>
-      </c>
-      <c r="G25" s="4">
+        <v>67</v>
+      </c>
+      <c r="G25" s="3">
         <v>175000</v>
       </c>
       <c r="H25" s="1">
@@ -2030,7 +2008,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2038,18 +2016,18 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>77</v>
+        <v>127</v>
       </c>
       <c r="D26" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E26" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F26" t="s">
-        <v>79</v>
-      </c>
-      <c r="G26" s="4">
+        <v>69</v>
+      </c>
+      <c r="G26" s="3">
         <v>185000</v>
       </c>
       <c r="H26" s="1">
@@ -2059,7 +2037,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2067,18 +2045,18 @@
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D27" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="E27" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F27" t="s">
-        <v>38</v>
-      </c>
-      <c r="G27" s="4">
+        <v>31</v>
+      </c>
+      <c r="G27" s="3">
         <v>195000</v>
       </c>
       <c r="H27" s="1">
@@ -2088,7 +2066,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2096,18 +2074,18 @@
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D28" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="E28" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F28" t="s">
-        <v>84</v>
-      </c>
-      <c r="G28" s="4">
+        <v>74</v>
+      </c>
+      <c r="G28" s="3">
         <v>205000</v>
       </c>
       <c r="H28" s="1">
@@ -2117,7 +2095,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2125,18 +2103,18 @@
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D29" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="E29" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F29" t="s">
-        <v>87</v>
-      </c>
-      <c r="G29" s="4">
+        <v>77</v>
+      </c>
+      <c r="G29" s="3">
         <v>225000</v>
       </c>
       <c r="H29" s="1">
@@ -2146,7 +2124,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9">
       <c r="A30">
         <v>27</v>
       </c>
@@ -2154,18 +2132,18 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D30" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="E30" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="F30" t="s">
-        <v>87</v>
-      </c>
-      <c r="G30" s="4">
+        <v>77</v>
+      </c>
+      <c r="G30" s="3">
         <v>225000</v>
       </c>
       <c r="H30" s="1">
@@ -2175,7 +2153,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9">
       <c r="A31">
         <v>28</v>
       </c>
@@ -2183,18 +2161,18 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D31" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E31" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F31" t="s">
-        <v>90</v>
-      </c>
-      <c r="G31" s="4">
+        <v>80</v>
+      </c>
+      <c r="G31" s="3">
         <v>235000</v>
       </c>
       <c r="H31" s="1">
@@ -2204,7 +2182,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9">
       <c r="A32">
         <v>29</v>
       </c>
@@ -2212,18 +2190,18 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D32" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E32" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F32" t="s">
-        <v>38</v>
-      </c>
-      <c r="G32" s="4">
+        <v>31</v>
+      </c>
+      <c r="G32" s="3">
         <v>245000</v>
       </c>
       <c r="H32" s="1">
@@ -2233,7 +2211,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9">
       <c r="A33">
         <v>30</v>
       </c>
@@ -2241,18 +2219,18 @@
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="D33" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="E33" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F33" t="s">
-        <v>94</v>
-      </c>
-      <c r="G33" s="4">
+        <v>84</v>
+      </c>
+      <c r="G33" s="3">
         <v>255000</v>
       </c>
       <c r="H33" s="1">
@@ -2262,7 +2240,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9">
       <c r="A34">
         <v>31</v>
       </c>
@@ -2270,18 +2248,18 @@
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D34" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E34" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F34" t="s">
-        <v>97</v>
-      </c>
-      <c r="G34" s="4">
+        <v>87</v>
+      </c>
+      <c r="G34" s="3">
         <v>265000</v>
       </c>
       <c r="H34" s="1">
@@ -2291,7 +2269,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9">
       <c r="A35">
         <v>32</v>
       </c>
@@ -2299,18 +2277,18 @@
         <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="D35" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E35" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F35" t="s">
-        <v>38</v>
-      </c>
-      <c r="G35" s="4">
+        <v>31</v>
+      </c>
+      <c r="G35" s="3">
         <v>275000</v>
       </c>
       <c r="H35" s="1">
@@ -2320,7 +2298,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9">
       <c r="A36">
         <v>33</v>
       </c>
@@ -2328,18 +2306,18 @@
         <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D36" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="E36" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F36" t="s">
-        <v>102</v>
-      </c>
-      <c r="G36" s="4">
+        <v>92</v>
+      </c>
+      <c r="G36" s="3">
         <v>285000</v>
       </c>
       <c r="H36" s="1">
@@ -2349,7 +2327,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9">
       <c r="A37">
         <v>34</v>
       </c>
@@ -2357,18 +2335,18 @@
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="D37" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="E37" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F37" t="s">
-        <v>105</v>
-      </c>
-      <c r="G37" s="4">
+        <v>95</v>
+      </c>
+      <c r="G37" s="3">
         <v>295000</v>
       </c>
       <c r="H37" s="1">
@@ -2378,7 +2356,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9">
       <c r="A38">
         <v>35</v>
       </c>
@@ -2386,18 +2364,18 @@
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="D38" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="E38" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F38" t="s">
-        <v>38</v>
-      </c>
-      <c r="G38" s="4">
+        <v>31</v>
+      </c>
+      <c r="G38" s="3">
         <v>305000</v>
       </c>
       <c r="H38" s="1">
@@ -2407,7 +2385,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9">
       <c r="A39">
         <v>36</v>
       </c>
@@ -2415,18 +2393,18 @@
         <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="D39" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="E39" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F39" t="s">
-        <v>108</v>
-      </c>
-      <c r="G39" s="4">
+        <v>98</v>
+      </c>
+      <c r="G39" s="3">
         <v>315000</v>
       </c>
       <c r="H39" s="1">
@@ -2436,7 +2414,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9">
       <c r="A40">
         <v>37</v>
       </c>
@@ -2444,18 +2422,18 @@
         <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="D40" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="E40" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F40" t="s">
-        <v>38</v>
-      </c>
-      <c r="G40" s="4">
+        <v>31</v>
+      </c>
+      <c r="G40" s="3">
         <v>325000</v>
       </c>
       <c r="H40" s="1">
@@ -2465,7 +2443,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9">
       <c r="A41">
         <v>38</v>
       </c>
@@ -2473,18 +2451,18 @@
         <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D41" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="E41" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F41" t="s">
-        <v>113</v>
-      </c>
-      <c r="G41" s="4">
+        <v>103</v>
+      </c>
+      <c r="G41" s="3">
         <v>335000</v>
       </c>
       <c r="H41" s="1">
@@ -2494,7 +2472,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9">
       <c r="A42">
         <v>39</v>
       </c>
@@ -2502,18 +2480,18 @@
         <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="D42" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="E42" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F42" t="s">
-        <v>116</v>
-      </c>
-      <c r="G42" s="4">
+        <v>106</v>
+      </c>
+      <c r="G42" s="3">
         <v>345000</v>
       </c>
       <c r="H42" s="1">
@@ -2523,7 +2501,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9">
       <c r="A43">
         <v>40</v>
       </c>
@@ -2531,18 +2509,18 @@
         <v>41</v>
       </c>
       <c r="C43" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D43" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E43" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F43" t="s">
-        <v>118</v>
-      </c>
-      <c r="G43" s="4">
+        <v>108</v>
+      </c>
+      <c r="G43" s="3">
         <v>355000</v>
       </c>
       <c r="H43" s="1">
@@ -2552,7 +2530,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9">
       <c r="A44">
         <v>41</v>
       </c>
@@ -2560,18 +2538,18 @@
         <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="D44" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="E44" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F44" t="s">
-        <v>121</v>
-      </c>
-      <c r="G44" s="4">
+        <v>111</v>
+      </c>
+      <c r="G44" s="3">
         <v>365000</v>
       </c>
       <c r="H44" s="1">
@@ -2581,7 +2559,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9">
       <c r="A45">
         <v>42</v>
       </c>
@@ -2589,18 +2567,18 @@
         <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D45" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="E45" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F45" t="s">
-        <v>124</v>
-      </c>
-      <c r="G45" s="4">
+        <v>114</v>
+      </c>
+      <c r="G45" s="3">
         <v>375000</v>
       </c>
       <c r="H45" s="1">
@@ -2610,7 +2588,7 @@
         <v>40972</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9">
       <c r="A46">
         <v>43</v>
       </c>
@@ -2618,86 +2596,61 @@
         <v>44</v>
       </c>
       <c r="C46" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="D46" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="E46" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F46" t="s">
-        <v>127</v>
-      </c>
-      <c r="G46" s="4">
+        <v>117</v>
+      </c>
+      <c r="G46" s="3">
         <v>395000</v>
       </c>
-      <c r="H46" s="2">
-        <v>44391</v>
-      </c>
-      <c r="I46" s="2">
+      <c r="H46" s="1">
+        <v>44391</v>
+      </c>
+      <c r="I46" s="1">
         <v>43862</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9">
       <c r="A47">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B47">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D47" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="E47" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="F47" t="s">
-        <v>127</v>
-      </c>
-      <c r="G47" s="4">
-        <v>395000</v>
-      </c>
-      <c r="H47" s="2">
-        <v>44391</v>
-      </c>
-      <c r="I47" s="2">
+        <v>120</v>
+      </c>
+      <c r="G47" s="3">
+        <v>405000</v>
+      </c>
+      <c r="H47" s="1">
+        <v>44391</v>
+      </c>
+      <c r="I47" s="1">
         <v>43862</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <v>44</v>
-      </c>
-      <c r="B48">
-        <v>45</v>
-      </c>
-      <c r="C48" t="s">
-        <v>128</v>
-      </c>
-      <c r="D48" t="s">
-        <v>129</v>
-      </c>
-      <c r="E48" t="s">
-        <v>132</v>
-      </c>
-      <c r="F48" t="s">
-        <v>130</v>
-      </c>
-      <c r="G48" s="4">
-        <v>405000</v>
-      </c>
-      <c r="H48" s="2">
-        <v>44391</v>
-      </c>
-      <c r="I48" s="2">
-        <v>43862</v>
-      </c>
+    <row r="48" spans="1:9">
+      <c r="G48"/>
     </row>
   </sheetData>
+  <autoFilter ref="E1:E48"/>
   <dataConsolidate/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>